<commit_message>
Better charts and references to them, abbreviated conclusions
</commit_message>
<xml_diff>
--- a/Charts/squared_error_11.xlsx
+++ b/Charts/squared_error_11.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27106"/>
-  <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yatharthdubey/Documents/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="28705"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="440" windowWidth="25600" windowHeight="14820" tabRatio="500"/>
+    <workbookView xWindow="5880" yWindow="600" windowWidth="25600" windowHeight="14820" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Chart1" sheetId="2" r:id="rId1"/>
@@ -18,11 +13,11 @@
   </sheets>
   <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
-    </ext>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
-      <mx:ArchID Flags="2"/>
     </ext>
   </extLst>
 </workbook>
@@ -644,14 +639,14 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2132440912"/>
-        <c:axId val="-2132433088"/>
+        <c:axId val="2111864440"/>
+        <c:axId val="2111250536"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2132440912"/>
+        <c:axId val="2111864440"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="100000.0"/>
+          <c:max val="40000.0"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
@@ -704,27 +699,8 @@
             </a:ln>
             <a:effectLst/>
           </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="2400" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="65000"/>
-                      <a:lumOff val="35000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="en-US"/>
-            </a:p>
-          </c:txPr>
         </c:title>
+        <c:numFmt formatCode="#,##0" sourceLinked="0"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -761,12 +737,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2132433088"/>
+        <c:crossAx val="2111250536"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2132433088"/>
+        <c:axId val="2111250536"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="0.1"/>
@@ -823,26 +799,6 @@
             </a:ln>
             <a:effectLst/>
           </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="2400" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="65000"/>
-                      <a:lumOff val="35000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="en-US"/>
-            </a:p>
-          </c:txPr>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
@@ -881,7 +837,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2132440912"/>
+        <c:crossAx val="2111864440"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1158,14 +1114,14 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2133000400"/>
-        <c:axId val="-2132461536"/>
+        <c:axId val="2113189400"/>
+        <c:axId val="2113196536"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2133000400"/>
+        <c:axId val="2113189400"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="100000.0"/>
+          <c:max val="40000.0"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
@@ -1223,27 +1179,8 @@
             </a:ln>
             <a:effectLst/>
           </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="2400" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="65000"/>
-                      <a:lumOff val="35000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="en-US"/>
-            </a:p>
-          </c:txPr>
         </c:title>
+        <c:numFmt formatCode="#,##0" sourceLinked="0"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -1280,12 +1217,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2132461536"/>
+        <c:crossAx val="2113196536"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2132461536"/>
+        <c:axId val="2113196536"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="2.0"/>
@@ -1342,26 +1279,6 @@
             </a:ln>
             <a:effectLst/>
           </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="2400" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="65000"/>
-                      <a:lumOff val="35000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="en-US"/>
-            </a:p>
-          </c:txPr>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
@@ -1400,7 +1317,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2133000400"/>
+        <c:crossAx val="2113189400"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2560,7 +2477,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="108" workbookViewId="0" zoomToFit="1"/>
+    <sheetView tabSelected="1" zoomScale="115" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -2571,7 +2488,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr/>
   <sheetViews>
-    <sheetView zoomScale="108" workbookViewId="0" zoomToFit="1"/>
+    <sheetView zoomScale="115" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -2582,7 +2499,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="8678333" cy="6291204"/>
+    <xdr:ext cx="8558696" cy="5819913"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1"/>
@@ -2609,7 +2526,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="8678333" cy="6291204"/>
+    <xdr:ext cx="8558696" cy="5819913"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1"/>
@@ -2675,7 +2592,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="Yu Gothic Light"/>
@@ -2710,7 +2627,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="Yu Gothic"/>
@@ -2887,7 +2804,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -3402,12 +3319,12 @@
   <dimension ref="A1:F22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCellId="1" sqref="F1:F1048576 A1:A1048576"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3427,7 +3344,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6">
       <c r="A2" s="1">
         <v>1000</v>
       </c>
@@ -3449,7 +3366,7 @@
         <v>1.1295965976596678</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6">
       <c r="A3" s="1">
         <v>6000</v>
       </c>
@@ -3471,7 +3388,7 @@
         <v>1.6410056977774261</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6">
       <c r="A4" s="1">
         <v>11000</v>
       </c>
@@ -3493,7 +3410,7 @@
         <v>2.0056734831534229</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6">
       <c r="A5" s="1">
         <v>16000</v>
       </c>
@@ -3515,7 +3432,7 @@
         <v>1.6554302291604026</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6">
       <c r="A6" s="1">
         <v>21000</v>
       </c>
@@ -3537,7 +3454,7 @@
         <v>1.5148838764868402</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:6">
       <c r="A7" s="1">
         <v>26000</v>
       </c>
@@ -3559,7 +3476,7 @@
         <v>1.4258751632148576</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:6">
       <c r="A8" s="1">
         <v>31000</v>
       </c>
@@ -3581,7 +3498,7 @@
         <v>1.2967830706033114</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:6">
       <c r="A9" s="1">
         <v>36000</v>
       </c>
@@ -3603,7 +3520,7 @@
         <v>1.3149562676536335</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:6">
       <c r="A10" s="1">
         <v>41000</v>
       </c>
@@ -3625,7 +3542,7 @@
         <v>1.2152184679554074</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:6">
       <c r="A11" s="1">
         <v>46000</v>
       </c>
@@ -3647,7 +3564,7 @@
         <v>1.1784328574999858</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:6">
       <c r="A12" s="1">
         <v>51000</v>
       </c>
@@ -3669,7 +3586,7 @@
         <v>1.1705410971324202</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:6">
       <c r="A13" s="1">
         <v>56000</v>
       </c>
@@ -3691,7 +3608,7 @@
         <v>1.2437203376192758</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:6">
       <c r="A14" s="1">
         <v>61000</v>
       </c>
@@ -3713,7 +3630,7 @@
         <v>1.0787308060548302</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:6">
       <c r="A15" s="1">
         <v>66000</v>
       </c>
@@ -3735,7 +3652,7 @@
         <v>1.1284805086277176</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:6">
       <c r="A16" s="1">
         <v>71000</v>
       </c>
@@ -3757,7 +3674,7 @@
         <v>1.1674368937932942</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:6">
       <c r="A17" s="1">
         <v>76000</v>
       </c>
@@ -3779,7 +3696,7 @@
         <v>1.1635369474219042</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:6">
       <c r="A18" s="1">
         <v>81000</v>
       </c>
@@ -3801,7 +3718,7 @@
         <v>1.1474426602113219</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:6">
       <c r="A19" s="1">
         <v>86000</v>
       </c>
@@ -3823,7 +3740,7 @@
         <v>1.1034588832478522</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:6">
       <c r="A20" s="1">
         <v>91000</v>
       </c>
@@ -3845,7 +3762,7 @@
         <v>1.1351971015263096</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:6">
       <c r="A21" s="1">
         <v>96000</v>
       </c>
@@ -3867,7 +3784,7 @@
         <v>1.1335943379706839</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:6">
       <c r="A22" s="1">
         <v>101000</v>
       </c>
@@ -3891,5 +3808,10 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>